<commit_message>
add initial conditions for bioreactors
</commit_message>
<xml_diff>
--- a/exposan/bsm2/data/data.xlsx
+++ b/exposan/bsm2/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yalin\Documents\Coding\EXPOsan\exposan\bsm2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5C98C2-4E8F-4352-BDFE-4D43C3A906BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9C64E5-B906-4FA4-A318-FD807937000E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5803" yWindow="2940" windowWidth="24831" windowHeight="14494" activeTab="1" xr2:uid="{7E1F8DB5-6AC0-49A5-80ED-764D72A7C198}"/>
+    <workbookView xWindow="8310" yWindow="2410" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{7E1F8DB5-6AC0-49A5-80ED-764D72A7C198}"/>
   </bookViews>
   <sheets>
     <sheet name="wastewater" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>Column19</t>
   </si>
@@ -241,6 +241,30 @@
   </si>
   <si>
     <t>AD1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>C1_s</t>
+  </si>
+  <si>
+    <t>C1_x</t>
+  </si>
+  <si>
+    <t>C1_tss</t>
   </si>
 </sst>
 </file>
@@ -290,7 +314,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -483,7 +527,7 @@
     <tableColumn id="12" xr3:uid="{2F7CCDC2-3934-423C-B07A-BC722E0A5EBD}" uniqueName="12" name="S_NH" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{43239465-D175-47CB-983F-D6B1D31085FC}" uniqueName="13" name="S_ND" queryTableFieldId="13"/>
     <tableColumn id="14" xr3:uid="{B97D679F-F19E-42F0-9C63-718DEA3BD3A0}" uniqueName="14" name="X_ND" queryTableFieldId="14"/>
-    <tableColumn id="15" xr3:uid="{C284D41F-69C1-499B-B257-EF06434E742D}" uniqueName="15" name="S_ALK" queryTableFieldId="15" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{C284D41F-69C1-499B-B257-EF06434E742D}" uniqueName="15" name="S_ALK" queryTableFieldId="15" dataDxfId="2"/>
     <tableColumn id="16" xr3:uid="{5CAF14B2-8DC5-4312-9461-9C12D2833BD8}" uniqueName="16" name="TSS" queryTableFieldId="16"/>
     <tableColumn id="17" xr3:uid="{1EA907AE-B10D-4763-BC90-16DCED7A462B}" uniqueName="17" name="Q" queryTableFieldId="17"/>
     <tableColumn id="18" xr3:uid="{1529FA29-85AF-4383-A77D-7F8A7470C017}" uniqueName="18" name="Temp" queryTableFieldId="18"/>
@@ -800,13 +844,13 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -874,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -943,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -1022,14 +1066,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53D8A14-0C34-4382-90B2-681B4FD651C1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>28.064299999999999</v>
+      </c>
+      <c r="C2">
+        <v>3.0503</v>
+      </c>
+      <c r="D2">
+        <v>1532.3</v>
+      </c>
+      <c r="E2">
+        <v>63.043300000000002</v>
+      </c>
+      <c r="F2">
+        <v>2245.1</v>
+      </c>
+      <c r="G2">
+        <v>166.66990000000001</v>
+      </c>
+      <c r="H2">
+        <v>964.89919999999995</v>
+      </c>
+      <c r="I2">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="J2">
+        <v>3.9350000000000001</v>
+      </c>
+      <c r="K2">
+        <v>6.8924000000000003</v>
+      </c>
+      <c r="L2">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="M2">
+        <v>3.8452999999999999</v>
+      </c>
+      <c r="N2">
+        <f>5.4213*12</f>
+        <v>65.055599999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>28.064299999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.3411999999999999</v>
+      </c>
+      <c r="D3">
+        <v>1532.3</v>
+      </c>
+      <c r="E3">
+        <v>58.857900000000001</v>
+      </c>
+      <c r="F3">
+        <v>2245.4</v>
+      </c>
+      <c r="G3">
+        <v>166.55119999999999</v>
+      </c>
+      <c r="H3">
+        <v>965.68050000000005</v>
+      </c>
+      <c r="I3">
+        <v>1.0907E-4</v>
+      </c>
+      <c r="J3">
+        <v>2.2206999999999999</v>
+      </c>
+      <c r="K3">
+        <v>7.2027999999999999</v>
+      </c>
+      <c r="L3">
+        <v>0.68620000000000003</v>
+      </c>
+      <c r="M3">
+        <v>3.7423999999999999</v>
+      </c>
+      <c r="N3">
+        <f>5.5659*12</f>
+        <v>66.790800000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <v>28.064299999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.95530000000000004</v>
+      </c>
+      <c r="D4">
+        <v>1532.3</v>
+      </c>
+      <c r="E4">
+        <v>46.298299999999998</v>
+      </c>
+      <c r="F4">
+        <v>2246.8000000000002</v>
+      </c>
+      <c r="G4">
+        <v>167.30770000000001</v>
+      </c>
+      <c r="H4">
+        <v>967.24419999999998</v>
+      </c>
+      <c r="I4">
+        <v>0.46629999999999999</v>
+      </c>
+      <c r="J4">
+        <v>5.5141</v>
+      </c>
+      <c r="K4">
+        <v>3.4247000000000001</v>
+      </c>
+      <c r="L4">
+        <v>0.65129999999999999</v>
+      </c>
+      <c r="M4">
+        <v>3.1404999999999998</v>
+      </c>
+      <c r="N4">
+        <f>5.0608*12</f>
+        <v>60.729600000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>28.064299999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.78059999999999996</v>
+      </c>
+      <c r="D5">
+        <v>1532.3</v>
+      </c>
+      <c r="E5">
+        <v>37.388100000000001</v>
+      </c>
+      <c r="F5">
+        <v>2245.6</v>
+      </c>
+      <c r="G5">
+        <v>167.8339</v>
+      </c>
+      <c r="H5">
+        <v>968.80719999999997</v>
+      </c>
+      <c r="I5">
+        <v>1.4283999999999999</v>
+      </c>
+      <c r="J5">
+        <v>8.4065999999999992</v>
+      </c>
+      <c r="K5">
+        <v>0.69220000000000004</v>
+      </c>
+      <c r="L5">
+        <v>0.60940000000000005</v>
+      </c>
+      <c r="M5">
+        <v>2.6815000000000002</v>
+      </c>
+      <c r="N5">
+        <f>4.659*12</f>
+        <v>55.908000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>28.064299999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.6734</v>
+      </c>
+      <c r="D6">
+        <v>1532.3</v>
+      </c>
+      <c r="E6">
+        <v>31.914400000000001</v>
+      </c>
+      <c r="F6">
+        <v>2242.1</v>
+      </c>
+      <c r="G6">
+        <v>167.84819999999999</v>
+      </c>
+      <c r="H6">
+        <v>970.36779999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.3748</v>
+      </c>
+      <c r="J6">
+        <v>9.1948000000000008</v>
+      </c>
+      <c r="K6">
+        <v>0.1585</v>
+      </c>
+      <c r="L6">
+        <v>0.55940000000000001</v>
+      </c>
+      <c r="M6">
+        <v>2.3925999999999998</v>
+      </c>
+      <c r="N6">
+        <f>4.5646*12</f>
+        <v>54.775200000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1042,9 +1368,9 @@
       <selection activeCell="AN1" sqref="AN1:AR1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>22</v>
       </c>
@@ -1175,7 +1501,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>63</v>
       </c>

</xml_diff>